<commit_message>
some changes to generate report
</commit_message>
<xml_diff>
--- a/src/test/resources/TestResource/excelwrite.xlsx
+++ b/src/test/resources/TestResource/excelwrite.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>success</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>812840410D</t>
+  </si>
+  <si>
+    <t>29Z13X5ZT4</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +1365,7 @@
     </row>
     <row r="6">
       <c r="H6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7">

</xml_diff>